<commit_message>
implementado el Whatsapp web
</commit_message>
<xml_diff>
--- a/data/registros.xlsx
+++ b/data/registros.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,6 +545,16 @@
       <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Ruta de carpeta</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>WhatsApp Profesional</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>WhatsApp Tramitador</t>
         </is>
       </c>
     </row>
@@ -559,7 +569,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,6 +653,16 @@
           <t>Ruta de carpeta</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>WhatsApp Profesional</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>WhatsApp Tramitador</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>